<commit_message>
Adding results to architecture table and getting figure headings for thesis
</commit_message>
<xml_diff>
--- a/ArchitectureResults.xlsx
+++ b/ArchitectureResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annarienbester/git/gravitationallenses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ADB6C38-0CAE-ED4D-9B6A-72883F75A449}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29409045-C7DB-C549-9ACF-7FBBD3ED211E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45700" yWindow="-1600" windowWidth="28040" windowHeight="17040" xr2:uid="{732A71FF-1E05-B648-932B-29EDA13B68A3}"/>
+    <workbookView xWindow="760" yWindow="960" windowWidth="28040" windowHeight="17040" xr2:uid="{732A71FF-1E05-B648-932B-29EDA13B68A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="42">
   <si>
     <t>DATE</t>
   </si>
@@ -148,16 +148,45 @@
   </si>
   <si>
     <t>28_10_2020_13_28_45</t>
+  </si>
+  <si>
+    <t>TIME TAKEN</t>
+  </si>
+  <si>
+    <t>142 minutes</t>
+  </si>
+  <si>
+    <t>28_10_2020_16_48_54</t>
+  </si>
+  <si>
+    <t>batch_size = 1024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -193,7 +222,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -210,20 +239,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Warning Text" xfId="2" builtinId="11"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -535,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E93F6C7-E908-4D48-BE36-12E94BF6CA1A}">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:N55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="93.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -546,226 +590,401 @@
     <col min="1" max="1" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="91" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="93.33203125" style="1"/>
+    <col min="4" max="4" width="18" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="93.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B3" s="4" t="s">
+      <c r="D2" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B4" s="4" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B5" s="4" t="s">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B6" s="4" t="s">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B7" s="4" t="s">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B8" s="4" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B9" s="4" t="s">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B10" s="4" t="s">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B11" s="4" t="s">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B12" s="4" t="s">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="4"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B13" s="4" t="s">
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="4"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B14" s="4" t="s">
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="4"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B15" s="4" t="s">
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="4"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B16" s="4" t="s">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="4"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B17" s="4" t="s">
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="4"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B18" s="4" t="s">
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="4"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B19" s="4" t="s">
+      <c r="C18" s="3"/>
+      <c r="D18" s="7"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="4"/>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B20" s="4" t="s">
+      <c r="C19" s="3"/>
+      <c r="D19" s="7"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="4"/>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B21" s="4" t="s">
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="4"/>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B22" s="4" t="s">
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="4"/>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B23" s="4" t="s">
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="4"/>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B24" s="4" t="s">
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B24" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="4"/>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B25" s="4" t="s">
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="4"/>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B26" s="4" t="s">
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B26" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="4"/>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B27" s="4" t="s">
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B27" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="4"/>
-    </row>
-    <row r="28" spans="2:3" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="5" t="s">
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:5" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="5"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B31" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B32" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B33" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B34" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B35" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B36" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B37" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B38" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B39" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B40" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B41" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B42" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B43" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B44" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B45" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B46" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B47" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B48" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B49" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B50" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B51" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B52" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B53" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B54" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding Results of the different architectures.
</commit_message>
<xml_diff>
--- a/ArchitectureResults.xlsx
+++ b/ArchitectureResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annarienbester/git/gravitationallenses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29409045-C7DB-C549-9ACF-7FBBD3ED211E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D32ADB-CDCB-0B4A-834A-C8156BC0D683}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="960" windowWidth="28040" windowHeight="17040" xr2:uid="{732A71FF-1E05-B648-932B-29EDA13B68A3}"/>
+    <workbookView xWindow="8280" yWindow="460" windowWidth="20380" windowHeight="17540" xr2:uid="{732A71FF-1E05-B648-932B-29EDA13B68A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="58">
   <si>
     <t>DATE</t>
   </si>
@@ -117,18 +117,6 @@
     <t>TEST LOSS</t>
   </si>
   <si>
-    <t>TEST LENS PREDICTED</t>
-  </si>
-  <si>
-    <t>TEST NO LENS PREDICTED</t>
-  </si>
-  <si>
-    <t>UNSEEN PREDICTED</t>
-  </si>
-  <si>
-    <t>UNSEEN NO PREDICTED</t>
-  </si>
-  <si>
     <t>TEST MEAN</t>
   </si>
   <si>
@@ -150,16 +138,76 @@
     <t>28_10_2020_13_28_45</t>
   </si>
   <si>
-    <t>TIME TAKEN</t>
-  </si>
-  <si>
-    <t>142 minutes</t>
-  </si>
-  <si>
-    <t>28_10_2020_16_48_54</t>
-  </si>
-  <si>
-    <t>batch_size = 1024</t>
+    <t>    #classifier.add(Conv2D(1024, (3, 3), activation='relu', padding='same'))</t>
+  </si>
+  <si>
+    <t>classifier.compile(optimizer=opt,</t>
+  </si>
+  <si>
+    <t>0.9767152667045593</t>
+  </si>
+  <si>
+    <t>0.06428686529397964</t>
+  </si>
+  <si>
+    <t>96.604243516922</t>
+  </si>
+  <si>
+    <t>1.3880060340693023</t>
+  </si>
+  <si>
+    <t>31.084338128566742</t>
+  </si>
+  <si>
+    <t>11.18342391587071</t>
+  </si>
+  <si>
+    <t>CONFUSION MATRIX UNSEEN</t>
+  </si>
+  <si>
+    <t>CONFUSION MATRIX TEST</t>
+  </si>
+  <si>
+    <t>[[5761  273]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [   8 6026]] </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> True Negative: 5761 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">False Positive: 273 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">False Negative: 8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">True Positive: 6026 </t>
+  </si>
+  <si>
+    <t>[[ 0  0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [62 21]] </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> True Negative: 0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">False Positive: 0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">False Negative: 62 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">True Positive: 21 </t>
+  </si>
+  <si>
+    <t>15,989,057</t>
+  </si>
+  <si>
+    <t>29_10_2020_14_31_10</t>
   </si>
 </sst>
 </file>
@@ -180,13 +228,6 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -213,13 +254,26 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF89890"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -249,28 +303,65 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Warning Text" xfId="2" builtinId="11"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF89890"/>
+      <color rgb="FFFA836F"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -579,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E93F6C7-E908-4D48-BE36-12E94BF6CA1A}">
-  <dimension ref="A1:N55"/>
+  <dimension ref="A1:K55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="93.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -590,21 +681,18 @@
     <col min="1" max="1" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="91" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="93.33203125" style="1"/>
+    <col min="4" max="4" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="93.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -612,22 +700,22 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>29</v>
@@ -636,357 +724,387 @@
         <v>30</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="M1" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="3"/>
-      <c r="D18" s="7"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="3"/>
-      <c r="D19" s="7"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="6"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D24" s="6"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-    </row>
-    <row r="28" spans="1:5" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:4" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B29" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B30" s="3" t="s">
+      <c r="C29" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B30" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B31" s="3" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B31" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B32" s="3" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B32" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B42" s="3" t="s">
-        <v>13</v>
+      <c r="B42" s="9" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B53" s="3" t="s">
-        <v>21</v>
+      <c r="B53" s="7" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="55" spans="2:2" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="8" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="top10" dxfId="2" priority="3" rank="5"/>
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D49">
+    <cfRule type="top10" dxfId="0" priority="1" rank="5"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixing KerasCNN for hep
</commit_message>
<xml_diff>
--- a/ArchitectureResults.xlsx
+++ b/ArchitectureResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annarienbester/git/gravitationallenses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D32ADB-CDCB-0B4A-834A-C8156BC0D683}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD505D1B-D6C2-2E4E-8A8C-2E9B850C9AF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8280" yWindow="460" windowWidth="20380" windowHeight="17540" xr2:uid="{732A71FF-1E05-B648-932B-29EDA13B68A3}"/>
   </bookViews>
@@ -673,7 +673,7 @@
   <dimension ref="A1:K55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="93.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fixing the KerasCNN.py to include a new architecture spreadsheet
</commit_message>
<xml_diff>
--- a/ArchitectureResults.xlsx
+++ b/ArchitectureResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annarienbester/git/gravitationallenses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD505D1B-D6C2-2E4E-8A8C-2E9B850C9AF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822A74A0-8C80-1B47-946F-56BDE015D804}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8280" yWindow="460" windowWidth="20380" windowHeight="17540" xr2:uid="{732A71FF-1E05-B648-932B-29EDA13B68A3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="60">
   <si>
     <t>DATE</t>
   </si>
@@ -207,7 +207,13 @@
     <t>15,989,057</t>
   </si>
   <si>
-    <t>29_10_2020_14_31_10</t>
+    <t>29_10_2020_15_15_18</t>
+  </si>
+  <si>
+    <t>29_10_2020_15_12_06</t>
+  </si>
+  <si>
+    <t>    #classifier.add(Conv2D(512, (3, 3), padding='same', activation='relu'))</t>
   </si>
 </sst>
 </file>
@@ -323,7 +329,17 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -670,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E93F6C7-E908-4D48-BE36-12E94BF6CA1A}">
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:K82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="93.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -951,7 +967,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>1</v>
@@ -1055,45 +1071,184 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B49" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B50" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B51" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B52" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B53" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B54" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="2:2" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B55" s="8" t="s">
         <v>23</v>
       </c>
     </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C56" s="7"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B57" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B58" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B59" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B60" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B61" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B62" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B63" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B64" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B65" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B66" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B67" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B68" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B69" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B70" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B71" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B72" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B73" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B74" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B75" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B76" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B77" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B78" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B79" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B80" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B81" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B82" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="top10" dxfId="2" priority="3" rank="5"/>
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="D1:D55 D83:D1048576">
+    <cfRule type="top10" dxfId="3" priority="6" rank="5"/>
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1103,6 +1258,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D49">
+    <cfRule type="top10" dxfId="2" priority="4" rank="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D56:D82">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="top10" dxfId="1" priority="3" rank="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D56:D76">
     <cfRule type="top10" dxfId="0" priority="1" rank="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding KerasCnn files to test architecture with
</commit_message>
<xml_diff>
--- a/ArchitectureResults.xlsx
+++ b/ArchitectureResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annarienbester/git/gravitationallenses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822A74A0-8C80-1B47-946F-56BDE015D804}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6986E61C-9D8C-A348-8A29-83E7508C1690}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8280" yWindow="460" windowWidth="20380" windowHeight="17540" xr2:uid="{732A71FF-1E05-B648-932B-29EDA13B68A3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="61">
   <si>
     <t>DATE</t>
   </si>
@@ -210,10 +210,13 @@
     <t>29_10_2020_15_15_18</t>
   </si>
   <si>
-    <t>29_10_2020_15_12_06</t>
-  </si>
-  <si>
     <t>    #classifier.add(Conv2D(512, (3, 3), padding='same', activation='relu'))</t>
+  </si>
+  <si>
+    <t>8,255,297</t>
+  </si>
+  <si>
+    <t>29_10_2020_16_21_25</t>
   </si>
 </sst>
 </file>
@@ -223,7 +226,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -266,6 +269,12 @@
       <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -313,7 +322,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -324,6 +333,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -688,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E93F6C7-E908-4D48-BE36-12E94BF6CA1A}">
   <dimension ref="A1:K82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="93.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -967,7 +977,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>1</v>
@@ -1113,7 +1123,9 @@
       <c r="B56" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C56" s="7"/>
+      <c r="C56" s="10" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B57" s="7" t="s">
@@ -1172,7 +1184,7 @@
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B68" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Getting files to run on hep, and plotkfold in execute k fold function
</commit_message>
<xml_diff>
--- a/ArchitectureResults.xlsx
+++ b/ArchitectureResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annarienbester/git/gravitationallenses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68516FD-CA8A-5A4C-810C-5699B7CD0C39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6366FA4E-5281-D140-BF88-8ED93ACE3436}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8280" yWindow="460" windowWidth="20380" windowHeight="17540" xr2:uid="{732A71FF-1E05-B648-932B-29EDA13B68A3}"/>
   </bookViews>
@@ -207,16 +207,16 @@
     <t>15,989,057</t>
   </si>
   <si>
-    <t>29_10_2020_15_15_18</t>
-  </si>
-  <si>
     <t>    #classifier.add(Conv2D(512, (3, 3), padding='same', activation='relu'))</t>
   </si>
   <si>
     <t>8,255,297</t>
   </si>
   <si>
-    <t>29_10_2020_16_21_25</t>
+    <t>29_10_2020_19_56_42</t>
+  </si>
+  <si>
+    <t>29_10_2020_19_57_39</t>
   </si>
 </sst>
 </file>
@@ -698,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E93F6C7-E908-4D48-BE36-12E94BF6CA1A}">
   <dimension ref="A1:K82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="93.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -977,7 +977,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>1</v>
@@ -1118,13 +1118,13 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B56" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -1184,7 +1184,7 @@
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B68" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added original data augmentation back to KerasCnn.py
</commit_message>
<xml_diff>
--- a/ArchitectureResults.xlsx
+++ b/ArchitectureResults.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annarienbester/git/gravitationallenses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2C4154-828E-4B4A-9EE1-78512F411B65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69393FCA-4973-0840-84AE-B9DECA4BD6EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8280" yWindow="460" windowWidth="20380" windowHeight="17540" xr2:uid="{732A71FF-1E05-B648-932B-29EDA13B68A3}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{732A71FF-1E05-B648-932B-29EDA13B68A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="76">
   <si>
     <t>DATE</t>
   </si>
@@ -144,24 +144,6 @@
     <t>classifier.compile(optimizer=opt,</t>
   </si>
   <si>
-    <t>0.9767152667045593</t>
-  </si>
-  <si>
-    <t>0.06428686529397964</t>
-  </si>
-  <si>
-    <t>96.604243516922</t>
-  </si>
-  <si>
-    <t>1.3880060340693023</t>
-  </si>
-  <si>
-    <t>31.084338128566742</t>
-  </si>
-  <si>
-    <t>11.18342391587071</t>
-  </si>
-  <si>
     <t>CONFUSION MATRIX UNSEEN</t>
   </si>
   <si>
@@ -213,10 +195,73 @@
     <t>8,255,297</t>
   </si>
   <si>
-    <t>29_10_2020_19_56_42</t>
-  </si>
-  <si>
-    <t>29_10_2020_19_57_39</t>
+    <t>30_10_2020_07_28_07</t>
+  </si>
+  <si>
+    <t>30_10_2020_07_28_38</t>
+  </si>
+  <si>
+    <t>[[5943   91]</t>
+  </si>
+  <si>
+    <t> [  48 5986]]</t>
+  </si>
+  <si>
+    <t>True Positive: 5986</t>
+  </si>
+  <si>
+    <t>False Negative: 48</t>
+  </si>
+  <si>
+    <t>False Positive: 91</t>
+  </si>
+  <si>
+    <t>True Negative: 5943</t>
+  </si>
+  <si>
+    <t>[[ 0  0]</t>
+  </si>
+  <si>
+    <t> [69 14]]</t>
+  </si>
+  <si>
+    <t>True Positive: 14</t>
+  </si>
+  <si>
+    <t>False Negative: 69</t>
+  </si>
+  <si>
+    <t>False Positive: 0</t>
+  </si>
+  <si>
+    <t>True Negative: 0</t>
+  </si>
+  <si>
+    <t>    opt = Adam(lr=learning_rate)  # lr = learning rate</t>
+  </si>
+  <si>
+    <t>    #classifier.add(Flatten())  # This is added before dense layer a flatten is needed</t>
+  </si>
+  <si>
+    <t>    #classifier.add(Dense(units=1024, activation='relu'))  # added new dense layer</t>
+  </si>
+  <si>
+    <t>    classifier.add(Dropout(0.2))  # antes era 0.25  </t>
+  </si>
+  <si>
+    <t>    classifier.add(Dropout(0.2))   </t>
+  </si>
+  <si>
+    <t>30_10_2020_10_44_44</t>
+  </si>
+  <si>
+    <t>UNSEEN LOSS</t>
+  </si>
+  <si>
+    <t>UNSEEN ACCURACY</t>
+  </si>
+  <si>
+    <t>7,205,697</t>
   </si>
 </sst>
 </file>
@@ -339,7 +384,167 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="20">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -696,10 +901,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E93F6C7-E908-4D48-BE36-12E94BF6CA1A}">
-  <dimension ref="A1:K82"/>
+  <dimension ref="A1:M109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="93.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -707,18 +912,20 @@
     <col min="1" max="1" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="91" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="93.33203125" style="1"/>
+    <col min="9" max="10" width="22.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="54" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="93.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -741,19 +948,25 @@
         <v>28</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="I1" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M1" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
@@ -763,140 +976,143 @@
       <c r="C2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="D2" s="1">
+        <v>0.97671526670455899</v>
+      </c>
+      <c r="E2" s="1">
+        <v>6.4286865293979603E-2</v>
+      </c>
+      <c r="F2" s="1">
+        <v>96.604243516921997</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1.3880060340692999</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" s="1">
+        <v>31.084338128566699</v>
+      </c>
+      <c r="K2" s="1">
+        <v>31.084338128566699</v>
+      </c>
+      <c r="L2" s="1">
+        <v>11.1834239158707</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="3"/>
       <c r="H3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="3"/>
       <c r="H4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="3"/>
       <c r="H5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="3"/>
       <c r="H6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="3"/>
       <c r="H7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
         <v>7</v>
       </c>
@@ -977,13 +1193,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -1081,210 +1297,401 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B49" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B50" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B51" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B52" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B53" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B54" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="1:3" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B55" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B56" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C56" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C56" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D56" s="7">
+        <v>0.98848193883895796</v>
+      </c>
+      <c r="E56" s="7">
+        <v>3.37656438350677E-2</v>
+      </c>
+      <c r="H56" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="I56" s="7">
+        <v>8.7758903503417898</v>
+      </c>
+      <c r="J56" s="7">
+        <v>16.8674692511558</v>
+      </c>
+      <c r="M56" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B57" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H57" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="I57" s="7"/>
+      <c r="J57" s="7"/>
+      <c r="M57" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B58" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B59" s="7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H59" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="I59" s="7"/>
+      <c r="J59" s="7"/>
+      <c r="M59" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B60" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B61" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H61" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I61" s="7"/>
+      <c r="J61" s="7"/>
+      <c r="M61" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B62" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B63" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="H63" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I63" s="7"/>
+      <c r="J63" s="7"/>
+      <c r="M63" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B64" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B65" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="H65" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="I65" s="7"/>
+      <c r="J65" s="7"/>
+      <c r="M65" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="66" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B66" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B67" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B68" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="69" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B69" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B70" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B71" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B72" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B73" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B74" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B75" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B76" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B77" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B78" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B79" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B80" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B81" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="82" spans="2:2" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B82" s="8" t="s">
         <v>23</v>
       </c>
     </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C83" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B84" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B85" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B86" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B87" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B88" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B89" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B90" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B91" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B92" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B93" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B94" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B95" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B96" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B97" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B98" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B99" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B100" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B101" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="102" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B102" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B103" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="104" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B104" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="105" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B105" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B106" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="107" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B107" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="108" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B108" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="109" spans="2:2" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B109" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D55 D83:D1048576">
-    <cfRule type="top10" dxfId="3" priority="6" rank="5"/>
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF0000"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D49">
-    <cfRule type="top10" dxfId="2" priority="4" rank="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D56:D82">
+  <conditionalFormatting sqref="D1:D1048576">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FFFF0000"/>
-        <color rgb="FF00B050"/>
+        <color rgb="FFFA836F"/>
+        <color theme="9" tint="0.39997558519241921"/>
       </colorScale>
     </cfRule>
-    <cfRule type="top10" dxfId="1" priority="3" rank="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D56:D76">
-    <cfRule type="top10" dxfId="0" priority="1" rank="5"/>
+  <conditionalFormatting sqref="J1:J1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF89890"/>
+        <color theme="9" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Got a test accuracy run that might work
</commit_message>
<xml_diff>
--- a/ArchitectureResults.xlsx
+++ b/ArchitectureResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annarienbester/git/gravitationallenses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7812340F-EB6E-E74A-9FEC-752FB063A651}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0529F66-931D-914B-8923-1308BDC311FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{732A71FF-1E05-B648-932B-29EDA13B68A3}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{732A71FF-1E05-B648-932B-29EDA13B68A3}"/>
   </bookViews>
   <sheets>
     <sheet name="OnHep" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="225">
   <si>
     <t>DATE</t>
   </si>
@@ -580,7 +580,136 @@
     <t>30_10_2020_16_12_48</t>
   </si>
   <si>
-    <t>30_10_2020_16_15_21</t>
+    <t>8.059048049926758</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>[[2000    0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [2000    0]] </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">True Positive: 0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">False Negative: 2000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">True Negative: 2000 </t>
+  </si>
+  <si>
+    <t>16.11809730529785</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [83  0]] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">False Negative: 83 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">True Negative: 0 </t>
+  </si>
+  <si>
+    <t># classifier.add(Flatten())  # This is added before dense layer a flatten is needed</t>
+  </si>
+  <si>
+    <t># classifier.add(Dense(units=1024, activation='relu'))  # added new dense layer</t>
+  </si>
+  <si>
+    <t>30_10_2020_17_33_51</t>
+  </si>
+  <si>
+    <t>76,411,713</t>
+  </si>
+  <si>
+    <t>30_10_2020_17_44_46</t>
+  </si>
+  <si>
+    <t>[[   0 6034]</t>
+  </si>
+  <si>
+    <t> [   0 6034]]</t>
+  </si>
+  <si>
+    <t>True Positive: 6034</t>
+  </si>
+  <si>
+    <t>False Negative: 0</t>
+  </si>
+  <si>
+    <t>False Positive: 6034</t>
+  </si>
+  <si>
+    <t> [ 0 83]]</t>
+  </si>
+  <si>
+    <t>True Positive: 83</t>
+  </si>
+  <si>
+    <t> 0,0</t>
+  </si>
+  <si>
+    <t> 0,5</t>
+  </si>
+  <si>
+    <t> 100,00</t>
+  </si>
+  <si>
+    <t>30_10_2020_17_56_32</t>
+  </si>
+  <si>
+    <t>Running with k = 5</t>
+  </si>
+  <si>
+    <t>To see what the accuracte results are</t>
+  </si>
+  <si>
+    <t>0.5829079480171203</t>
+  </si>
+  <si>
+    <t>0.80175</t>
+  </si>
+  <si>
+    <t>[[1273  727]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [  66 1934]] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">True Positive: 1934 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">False Negative: 66 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">False Positive: 727 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">True Negative: 1273 </t>
+  </si>
+  <si>
+    <t>1.0154433250427246</t>
+  </si>
+  <si>
+    <t>0.6987951993942261</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [25 58]] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">True Positive: 58 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">False Negative: 25 </t>
   </si>
 </sst>
 </file>
@@ -590,7 +719,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -640,6 +769,12 @@
       <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color theme="1"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -695,7 +830,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -705,12 +840,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -720,6 +849,17 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1041,13 +1181,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E93F6C7-E908-4D48-BE36-12E94BF6CA1A}">
-  <dimension ref="A1:M220"/>
+  <dimension ref="A1:M244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="B225" sqref="B225"/>
+    <sheetView tabSelected="1" topLeftCell="A203" zoomScale="92" workbookViewId="0">
+      <selection activeCell="C221" sqref="C221"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="93.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="93.33203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.1640625" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="91" style="6" bestFit="1" customWidth="1"/>
@@ -1065,89 +1205,89 @@
     <col min="15" max="16384" width="93.33203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13">
       <c r="B1" s="3" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13">
       <c r="B2" s="3" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13">
       <c r="B3" s="3" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13">
       <c r="B4" s="3" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13">
       <c r="B5" s="3" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13">
       <c r="B6" s="3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13">
       <c r="B7" s="3" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13">
       <c r="B8" s="3" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="8" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:13" s="13" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+    <row r="9" spans="1:13" s="8" customFormat="1" ht="16" thickBot="1"/>
+    <row r="10" spans="1:13" s="11" customFormat="1" ht="16" thickBot="1">
+      <c r="A10" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="H10" s="13" t="s">
+      <c r="H10" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="I10" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="J10" s="13" t="s">
+      <c r="J10" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="K10" s="13" t="s">
+      <c r="K10" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="L10" s="13" t="s">
+      <c r="L10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="M10" s="13" t="s">
+      <c r="M10" s="11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13">
       <c r="A11" s="6" t="s">
         <v>33</v>
       </c>
@@ -1185,7 +1325,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13">
       <c r="B12" s="3" t="s">
         <v>2</v>
       </c>
@@ -1197,7 +1337,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13">
       <c r="B13" s="3" t="s">
         <v>3</v>
       </c>
@@ -1209,7 +1349,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13">
       <c r="B14" s="3" t="s">
         <v>4</v>
       </c>
@@ -1221,7 +1361,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13">
       <c r="B15" s="3" t="s">
         <v>5</v>
       </c>
@@ -1233,7 +1373,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13">
       <c r="B16" s="3" t="s">
         <v>6</v>
       </c>
@@ -1245,134 +1385,134 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3">
       <c r="B17" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:3">
       <c r="B18" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:3">
       <c r="B19" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:3">
       <c r="B20" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:3">
       <c r="B21" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:3">
       <c r="B22" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:3">
       <c r="B23" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:3">
       <c r="B24" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:3">
       <c r="B25" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:3">
       <c r="B26" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:3">
       <c r="B27" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:3">
       <c r="B28" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C28" s="3"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:3">
       <c r="B29" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:3">
       <c r="B30" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:3">
       <c r="B31" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C31" s="3"/>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:3">
       <c r="B32" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13">
       <c r="B33" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C33" s="3"/>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13">
       <c r="B34" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13">
       <c r="B35" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C35" s="3"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13">
       <c r="B36" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="1:13" s="8" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" s="8" customFormat="1" ht="16" thickBot="1">
       <c r="B37" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C37" s="4"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13">
       <c r="A38" s="6" t="s">
         <v>53</v>
       </c>
@@ -1401,7 +1541,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13">
       <c r="B39" s="3" t="s">
         <v>2</v>
       </c>
@@ -1412,14 +1552,14 @@
         <v>155</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13">
       <c r="B40" s="3" t="s">
         <v>3</v>
       </c>
       <c r="H40" s="3"/>
       <c r="M40" s="3"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13">
       <c r="B41" s="3" t="s">
         <v>4</v>
       </c>
@@ -1430,14 +1570,14 @@
         <v>156</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" ht="16">
       <c r="B42" s="3" t="s">
         <v>5</v>
       </c>
       <c r="H42" s="1"/>
       <c r="M42" s="1"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13">
       <c r="B43" s="3" t="s">
         <v>6</v>
       </c>
@@ -1448,14 +1588,14 @@
         <v>157</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" ht="16">
       <c r="B44" s="3" t="s">
         <v>7</v>
       </c>
       <c r="H44" s="1"/>
       <c r="M44" s="1"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13">
       <c r="B45" s="3" t="s">
         <v>8</v>
       </c>
@@ -1466,14 +1606,14 @@
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" ht="16">
       <c r="B46" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H46" s="1"/>
       <c r="M46" s="1"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13">
       <c r="B47" s="3" t="s">
         <v>10</v>
       </c>
@@ -1484,92 +1624,92 @@
         <v>86</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13">
       <c r="B48" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:2">
       <c r="B49" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:2">
       <c r="B50" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:2">
       <c r="B51" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:2">
       <c r="B52" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:2">
       <c r="B53" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:2">
       <c r="B54" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:2">
       <c r="B55" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:2">
       <c r="B56" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:2">
       <c r="B57" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:2">
       <c r="B58" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:2">
       <c r="B59" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:2">
       <c r="B60" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:2">
       <c r="B61" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:2">
       <c r="B62" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:2">
       <c r="B63" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="64" spans="2:2" s="8" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:2" s="8" customFormat="1" ht="16" thickBot="1">
       <c r="B64" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13">
       <c r="A65" s="6" t="s">
         <v>54</v>
       </c>
@@ -1591,14 +1731,14 @@
       <c r="I65" s="3">
         <v>8.7758903503417898</v>
       </c>
-      <c r="J65" s="11">
+      <c r="J65" s="9">
         <v>16.8674692511558</v>
       </c>
       <c r="M65" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13">
       <c r="B66" s="3" t="s">
         <v>2</v>
       </c>
@@ -1611,12 +1751,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:13">
       <c r="B67" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:13">
       <c r="B68" s="3" t="s">
         <v>4</v>
       </c>
@@ -1629,12 +1769,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:13">
       <c r="B69" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:13">
       <c r="B70" s="3" t="s">
         <v>6</v>
       </c>
@@ -1647,12 +1787,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13">
       <c r="B71" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:13">
       <c r="B72" s="3" t="s">
         <v>8</v>
       </c>
@@ -1665,12 +1805,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:13">
       <c r="B73" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:13">
       <c r="B74" s="3" t="s">
         <v>10</v>
       </c>
@@ -1683,92 +1823,92 @@
         <v>66</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:13">
       <c r="B75" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:13">
       <c r="B76" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:13">
       <c r="B77" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:13">
       <c r="B78" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:13">
       <c r="B79" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:13">
       <c r="B80" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:13">
       <c r="B81" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:13">
       <c r="B82" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:13">
       <c r="B83" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:13">
       <c r="B84" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:13">
       <c r="B85" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:13">
       <c r="B86" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:13">
       <c r="B87" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:13">
       <c r="B88" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:13">
       <c r="B89" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:13">
       <c r="B90" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="91" spans="1:13" s="8" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" s="8" customFormat="1" ht="16" thickBot="1">
       <c r="B91" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:13">
       <c r="A92" s="3" t="s">
         <v>72</v>
       </c>
@@ -1797,7 +1937,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:13">
       <c r="B93" s="3" t="s">
         <v>2</v>
       </c>
@@ -1808,14 +1948,14 @@
         <v>82</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:13">
       <c r="B94" s="3" t="s">
         <v>3</v>
       </c>
       <c r="H94" s="3"/>
       <c r="M94" s="3"/>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:13">
       <c r="B95" s="3" t="s">
         <v>4</v>
       </c>
@@ -1826,12 +1966,12 @@
         <v>83</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:13">
       <c r="B96" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:13">
       <c r="B97" s="3" t="s">
         <v>6</v>
       </c>
@@ -1842,12 +1982,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="98" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:13">
       <c r="B98" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="99" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:13">
       <c r="B99" s="3" t="s">
         <v>8</v>
       </c>
@@ -1858,12 +1998,12 @@
         <v>85</v>
       </c>
     </row>
-    <row r="100" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:13">
       <c r="B100" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:13">
       <c r="B101" s="3" t="s">
         <v>10</v>
       </c>
@@ -1874,92 +2014,92 @@
         <v>86</v>
       </c>
     </row>
-    <row r="102" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:13">
       <c r="B102" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="103" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:13">
       <c r="B103" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="104" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:13">
       <c r="B104" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="105" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:13">
       <c r="B105" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="106" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:13">
       <c r="B106" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="107" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:13">
       <c r="B107" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="108" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:13">
       <c r="B108" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="109" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:13">
       <c r="B109" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="110" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:13">
       <c r="B110" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="111" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:13">
       <c r="B111" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="112" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:13">
       <c r="B112" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:13">
       <c r="B113" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:13">
       <c r="B114" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:13">
       <c r="B115" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:13">
       <c r="B116" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:13">
       <c r="B117" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="118" spans="1:13" s="8" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:13" s="8" customFormat="1" ht="16" thickBot="1">
       <c r="B118" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:13">
       <c r="A119" s="3" t="s">
         <v>88</v>
       </c>
@@ -1988,7 +2128,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:13">
       <c r="B120" s="3" t="s">
         <v>2</v>
       </c>
@@ -1999,8 +2139,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A121" s="10" t="s">
+    <row r="121" spans="1:13">
+      <c r="A121" s="21" t="s">
         <v>89</v>
       </c>
       <c r="B121" s="3" t="s">
@@ -2009,8 +2149,8 @@
       <c r="H121" s="3"/>
       <c r="M121" s="3"/>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A122" s="10"/>
+    <row r="122" spans="1:13">
+      <c r="A122" s="21"/>
       <c r="B122" s="3" t="s">
         <v>4</v>
       </c>
@@ -2021,15 +2161,15 @@
         <v>97</v>
       </c>
     </row>
-    <row r="123" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A123" s="10"/>
+    <row r="123" spans="1:13" ht="16">
+      <c r="A123" s="21"/>
       <c r="B123" s="3" t="s">
         <v>5</v>
       </c>
       <c r="H123" s="1"/>
       <c r="M123" s="1"/>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:13">
       <c r="B124" s="3" t="s">
         <v>6</v>
       </c>
@@ -2040,14 +2180,14 @@
         <v>98</v>
       </c>
     </row>
-    <row r="125" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:13" ht="16">
       <c r="B125" s="3" t="s">
         <v>7</v>
       </c>
       <c r="H125" s="1"/>
       <c r="M125" s="1"/>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:13">
       <c r="B126" s="3" t="s">
         <v>8</v>
       </c>
@@ -2058,14 +2198,14 @@
         <v>85</v>
       </c>
     </row>
-    <row r="127" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:13" ht="16">
       <c r="B127" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H127" s="1"/>
       <c r="M127" s="1"/>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:13">
       <c r="B128" s="3" t="s">
         <v>10</v>
       </c>
@@ -2076,92 +2216,92 @@
         <v>86</v>
       </c>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="129" spans="2:2">
       <c r="B129" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:2">
       <c r="B130" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="131" spans="2:2">
       <c r="B131" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="132" spans="2:2">
       <c r="B132" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="133" spans="2:2">
       <c r="B133" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="134" spans="2:2">
       <c r="B134" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="135" spans="2:2">
       <c r="B135" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="136" spans="2:2">
       <c r="B136" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="137" spans="2:2">
       <c r="B137" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="138" spans="2:2">
       <c r="B138" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="139" spans="2:2">
       <c r="B139" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="140" spans="2:2">
       <c r="B140" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="141" spans="2:2">
       <c r="B141" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="142" spans="2:2">
       <c r="B142" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="143" spans="2:2">
       <c r="B143" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="144" spans="2:2">
       <c r="B144" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="145" spans="1:13" s="8" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:13" s="8" customFormat="1" ht="16" thickBot="1">
       <c r="B145" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:13">
       <c r="A146" s="3" t="s">
         <v>111</v>
       </c>
@@ -2190,7 +2330,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:13">
       <c r="B147" s="3" t="s">
         <v>2</v>
       </c>
@@ -2201,14 +2341,14 @@
         <v>62</v>
       </c>
     </row>
-    <row r="148" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:13" ht="16">
       <c r="B148" s="3" t="s">
         <v>3</v>
       </c>
       <c r="H148" s="1"/>
       <c r="M148" s="1"/>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:13">
       <c r="B149" s="3" t="s">
         <v>4</v>
       </c>
@@ -2219,14 +2359,14 @@
         <v>63</v>
       </c>
     </row>
-    <row r="150" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:13" ht="16">
       <c r="B150" s="5" t="s">
         <v>99</v>
       </c>
       <c r="H150" s="1"/>
       <c r="M150" s="1"/>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:13">
       <c r="B151" s="5" t="s">
         <v>100</v>
       </c>
@@ -2237,14 +2377,14 @@
         <v>64</v>
       </c>
     </row>
-    <row r="152" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:13" ht="16">
       <c r="B152" s="5" t="s">
         <v>101</v>
       </c>
       <c r="H152" s="1"/>
       <c r="M152" s="1"/>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:13">
       <c r="B153" s="5" t="s">
         <v>102</v>
       </c>
@@ -2255,14 +2395,14 @@
         <v>65</v>
       </c>
     </row>
-    <row r="154" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:13" ht="16">
       <c r="B154" s="5" t="s">
         <v>103</v>
       </c>
       <c r="H154" s="1"/>
       <c r="M154" s="1"/>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:13">
       <c r="B155" s="5" t="s">
         <v>104</v>
       </c>
@@ -2273,348 +2413,549 @@
         <v>66</v>
       </c>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:13">
       <c r="B156" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:13">
       <c r="B157" s="5" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:13">
       <c r="B158" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:13">
       <c r="B159" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:13">
       <c r="B160" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:13">
       <c r="B161" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:13">
       <c r="B162" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:13">
       <c r="B163" s="5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:13">
       <c r="B164" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:13">
       <c r="B165" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:13">
       <c r="B166" s="5" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:13">
       <c r="B167" s="5" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:13">
       <c r="B168" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:13">
       <c r="B169" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:13">
       <c r="B170" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:13">
       <c r="B171" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="172" spans="1:2" s="8" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:13" s="8" customFormat="1" ht="16" thickBot="1">
       <c r="B172" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:13">
       <c r="A173" s="6" t="s">
         <v>180</v>
       </c>
       <c r="B173" s="3" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C173" s="3">
+        <v>37.889000000000003</v>
+      </c>
+      <c r="D173" s="3">
+        <v>7.6438503265380797</v>
+      </c>
+      <c r="E173" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H173" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="I173" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="J173" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="M173" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="174" spans="1:13">
       <c r="B174" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A175" s="9" t="s">
+      <c r="H174" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="M174" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="175" spans="1:13" ht="16">
+      <c r="A175" s="22" t="s">
         <v>172</v>
       </c>
       <c r="B175" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A176" s="9"/>
+      <c r="H175" s="1"/>
+      <c r="M175" s="1"/>
+    </row>
+    <row r="176" spans="1:13">
+      <c r="A176" s="22"/>
       <c r="B176" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="H176" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="M176" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="177" spans="2:13" ht="16">
       <c r="B177" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="H177" s="1"/>
+      <c r="M177" s="1"/>
+    </row>
+    <row r="178" spans="2:13">
       <c r="B178" s="5" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="179" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="H178" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="M178" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="179" spans="2:13" ht="16">
       <c r="B179" s="5" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="180" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="H179" s="1"/>
+      <c r="M179" s="1"/>
+    </row>
+    <row r="180" spans="2:13">
       <c r="B180" s="5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="H180" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="M180" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="181" spans="2:13" ht="16">
       <c r="B181" s="5" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="H181" s="1"/>
+      <c r="M181" s="1"/>
+    </row>
+    <row r="182" spans="2:13">
       <c r="B182" s="5" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="183" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="H182" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="M182" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="183" spans="2:13">
       <c r="B183" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="184" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="184" spans="2:13">
       <c r="B184" s="5" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="185" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="185" spans="2:13">
       <c r="B185" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="186" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="186" spans="2:13">
       <c r="B186" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="187" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="187" spans="2:13">
       <c r="B187" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="188" spans="2:13">
       <c r="B188" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="189" spans="2:13">
       <c r="B189" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="190" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="190" spans="2:13">
       <c r="B190" s="5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="191" spans="2:13">
       <c r="B191" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="192" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="192" spans="2:13">
       <c r="B192" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:3">
       <c r="B193" s="5" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:3">
       <c r="B194" s="5" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B195" s="17" t="s">
+    <row r="195" spans="1:3">
+      <c r="B195" s="15" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="196" spans="1:2" s="8" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" s="8" customFormat="1" ht="16" thickBot="1">
       <c r="B196" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A197" s="6" t="s">
-        <v>181</v>
+    <row r="197" spans="1:3">
+      <c r="A197" s="3" t="s">
+        <v>198</v>
       </c>
       <c r="B197" s="3" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="198" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C197" s="3">
+        <v>93.376999999999995</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" s="16" customFormat="1">
       <c r="B198" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="199" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B199" s="19" t="s">
+    <row r="199" spans="1:3" s="16" customFormat="1">
+      <c r="B199" s="17" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:3">
       <c r="B200" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:3">
       <c r="B201" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:3">
       <c r="B202" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:3">
       <c r="B203" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:3">
       <c r="B204" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:3">
       <c r="B205" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:3">
       <c r="B206" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:3">
       <c r="B207" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:3">
       <c r="B208" s="5" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="209" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:3">
       <c r="B209" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="210" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:3">
       <c r="B210" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="211" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:3">
       <c r="B211" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="212" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:3">
       <c r="B212" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="213" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:3">
       <c r="B213" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="214" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:3">
       <c r="B214" s="5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="215" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:3">
       <c r="B215" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="216" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:3">
       <c r="B216" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="217" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:3">
       <c r="B217" s="5" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="218" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:3">
       <c r="B218" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="219" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:3">
       <c r="B219" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="220" spans="2:2" s="8" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:3" s="8" customFormat="1" ht="16" thickBot="1">
       <c r="B220" s="4" t="s">
         <v>20</v>
       </c>
     </row>
+    <row r="221" spans="1:3">
+      <c r="A221" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="B221" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C221" s="3">
+        <v>37.889000000000003</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3">
+      <c r="B222" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3">
+      <c r="A223" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="B223" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3">
+      <c r="A224" s="22"/>
+      <c r="B224" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2">
+      <c r="B225" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2">
+      <c r="A226" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="B226" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2">
+      <c r="A227" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="B227" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2">
+      <c r="A228" s="22"/>
+      <c r="B228" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2">
+      <c r="B229" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2">
+      <c r="B230" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2">
+      <c r="B231" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2">
+      <c r="B232" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2">
+      <c r="B233" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2">
+      <c r="B234" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2">
+      <c r="B235" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2">
+      <c r="B236" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2">
+      <c r="B237" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2">
+      <c r="B238" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2">
+      <c r="B239" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2">
+      <c r="B240" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="241" spans="2:2">
+      <c r="B241" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="242" spans="2:2">
+      <c r="B242" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="243" spans="2:2">
+      <c r="B243" s="15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="244" spans="2:2" s="8" customFormat="1" ht="16" thickBot="1">
+      <c r="B244" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A121:A123"/>
     <mergeCell ref="A175:A176"/>
+    <mergeCell ref="A223:A224"/>
+    <mergeCell ref="A227:A228"/>
   </mergeCells>
-  <conditionalFormatting sqref="E10:E37 E93:E118 E120:E145 E157:E1048576 E39:E91">
-    <cfRule type="colorScale" priority="17">
+  <conditionalFormatting sqref="E10:E37 E93:E118 E120:E145 E157:E172 E39:E91 E174:E1048576">
+    <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2623,8 +2964,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E10:E37 E120:E145 E157:E1048576 E39:E118">
-    <cfRule type="colorScale" priority="22">
+  <conditionalFormatting sqref="E10:E37 E120:E145 E157:E172 E39:E118 E174:E1048576">
+    <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2632,7 +2973,7 @@
         <color rgb="FF92D050"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="23">
+    <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2643,8 +2984,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J11:J37 J157:J263 J39:J145">
-    <cfRule type="colorScale" priority="50">
+  <conditionalFormatting sqref="J11:J37 J157:J172 J39:J145 J174:J263">
+    <cfRule type="colorScale" priority="51">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2653,8 +2994,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J11:J802">
-    <cfRule type="colorScale" priority="54">
+  <conditionalFormatting sqref="J11:J172 J174:J802">
+    <cfRule type="colorScale" priority="55">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2663,13 +3004,23 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E11:E922">
-    <cfRule type="colorScale" priority="56">
+  <conditionalFormatting sqref="E11:E172 E174:E922">
+    <cfRule type="colorScale" priority="57">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
         <color rgb="FFF89890"/>
         <color theme="9" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J11:J1048576 J1:J9">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FF92D050"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -2679,260 +3030,497 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EF8B63F-B594-7045-961A-3C8367EEFC3D}">
-  <dimension ref="A1:M38"/>
+  <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="75.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="23" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13">
       <c r="B1" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13">
       <c r="B2" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13">
       <c r="B3" s="1" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13">
       <c r="B4" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13">
       <c r="B5" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13">
       <c r="B6" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13">
       <c r="B7" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13">
       <c r="B8" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:13" s="12" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+    <row r="9" spans="1:13" s="2" customFormat="1" ht="17" thickBot="1"/>
+    <row r="10" spans="1:13" s="10" customFormat="1" thickBot="1">
+      <c r="A10" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="H10" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="I10" s="12" t="s">
+      <c r="I10" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="J10" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="J10" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="K10" s="12" t="s">
+      <c r="K10" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="L10" s="12" t="s">
+      <c r="L10" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="M10" s="12" t="s">
+      <c r="M10" s="10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13">
       <c r="A11" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="12" t="s">
         <v>115</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B12" s="14" t="s">
+      <c r="D11" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="B12" s="12" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B13" s="14" t="s">
+      <c r="H12" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="B13" s="12" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B14" s="14" t="s">
+      <c r="H13" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="B14" s="12" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B15" s="14" t="s">
+      <c r="H14" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="B15" s="12" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B16" s="14" t="s">
+      <c r="H15" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="B16" s="12" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" s="14" t="s">
+      <c r="H16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13">
+      <c r="B17" s="12" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" s="14" t="s">
+      <c r="H17" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13">
+      <c r="B18" s="12" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B19" s="14" t="s">
+    <row r="19" spans="2:13">
+      <c r="B19" s="12" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B20" s="14" t="s">
+    <row r="20" spans="2:13">
+      <c r="B20" s="12" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B21" s="16" t="s">
+    <row r="21" spans="2:13">
+      <c r="B21" s="14" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B22" s="16" t="s">
+    <row r="22" spans="2:13">
+      <c r="B22" s="14" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B23" s="16" t="s">
+    <row r="23" spans="2:13">
+      <c r="B23" s="14" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B24" s="16" t="s">
+    <row r="24" spans="2:13">
+      <c r="B24" s="14" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B25" s="16" t="s">
+    <row r="25" spans="2:13">
+      <c r="B25" s="14" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B26" s="14" t="s">
+    <row r="26" spans="2:13">
+      <c r="B26" s="12" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B27" s="14" t="s">
+    <row r="27" spans="2:13">
+      <c r="B27" s="12" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B28" s="14" t="s">
+    <row r="28" spans="2:13">
+      <c r="B28" s="12" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B29" s="14" t="s">
+    <row r="29" spans="2:13">
+      <c r="B29" s="12" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B30" s="14" t="s">
+    <row r="30" spans="2:13">
+      <c r="B30" s="12" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B31" s="14" t="s">
+    <row r="31" spans="2:13">
+      <c r="B31" s="12" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B32" s="14" t="s">
+    <row r="32" spans="2:13">
+      <c r="B32" s="12" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B33" s="14" t="s">
+    <row r="33" spans="1:13">
+      <c r="B33" s="12" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B34" s="14" t="s">
+    <row r="34" spans="1:13">
+      <c r="B34" s="12" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B35" s="14" t="s">
+    <row r="35" spans="1:13">
+      <c r="B35" s="12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B36" s="14" t="s">
+    <row r="36" spans="1:13">
+      <c r="B36" s="12" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B37" s="14" t="s">
+    <row r="37" spans="1:13">
+      <c r="B37" s="12" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="38" spans="2:2" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="15" t="s">
+    <row r="38" spans="1:13" s="2" customFormat="1" ht="17" thickBot="1">
+      <c r="B38" s="13" t="s">
         <v>132</v>
       </c>
     </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B39" s="18"/>
+      <c r="C39" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="B40" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="B41" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="B42" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="B43" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="B44" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="B45" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="B46" s="19" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="B47" s="19" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="B48" s="19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49" s="19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50" s="20" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2">
+      <c r="B51" s="20" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2">
+      <c r="B52" s="20" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2">
+      <c r="B53" s="20" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2">
+      <c r="B54" s="20" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2">
+      <c r="B55" s="20" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2">
+      <c r="B56" s="20" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2">
+      <c r="B57" s="19" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2">
+      <c r="B58" s="19" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2">
+      <c r="B59" s="19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2">
+      <c r="B60" s="19" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2">
+      <c r="B61" s="19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2">
+      <c r="B62" s="19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" s="2" customFormat="1" ht="17" thickBot="1">
+      <c r="B63" s="24" t="s">
+        <v>114</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D10">
+  <conditionalFormatting sqref="E10">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -2942,7 +3530,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D10">
+  <conditionalFormatting sqref="E10">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Adding results to table, and then copied one that works onto hep
</commit_message>
<xml_diff>
--- a/ArchitectureResults.xlsx
+++ b/ArchitectureResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annarienbester/git/gravitationallenses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0529F66-931D-914B-8923-1308BDC311FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B71863-36C9-0C42-BC0E-66F5885904E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{732A71FF-1E05-B648-932B-29EDA13B68A3}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{732A71FF-1E05-B648-932B-29EDA13B68A3}"/>
   </bookViews>
   <sheets>
     <sheet name="OnHep" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="234">
   <si>
     <t>DATE</t>
   </si>
@@ -658,9 +658,6 @@
     <t> 0,0</t>
   </si>
   <si>
-    <t> 0,5</t>
-  </si>
-  <si>
     <t> 100,00</t>
   </si>
   <si>
@@ -676,9 +673,6 @@
     <t>0.5829079480171203</t>
   </si>
   <si>
-    <t>0.80175</t>
-  </si>
-  <si>
     <t>[[1273  727]</t>
   </si>
   <si>
@@ -700,9 +694,6 @@
     <t>1.0154433250427246</t>
   </si>
   <si>
-    <t>0.6987951993942261</t>
-  </si>
-  <si>
     <t xml:space="preserve"> [25 58]] </t>
   </si>
   <si>
@@ -710,6 +701,42 @@
   </si>
   <si>
     <t xml:space="preserve">False Negative: 25 </t>
+  </si>
+  <si>
+    <t> [  25 6009]]</t>
+  </si>
+  <si>
+    <t>True Positive: 6009</t>
+  </si>
+  <si>
+    <t>False Negative: 25</t>
+  </si>
+  <si>
+    <t>False Positive: 125</t>
+  </si>
+  <si>
+    <t>True Negative: 5909</t>
+  </si>
+  <si>
+    <t> [73 10]]</t>
+  </si>
+  <si>
+    <t>True Positive: 10</t>
+  </si>
+  <si>
+    <t>False Negative: 73</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>31_10_2020_07_24_19</t>
+  </si>
+  <si>
+    <t>Running the one from my laptop on hep, with k=5</t>
+  </si>
+  <si>
+    <t> 98,75704050064087</t>
   </si>
 </sst>
 </file>
@@ -719,7 +746,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -776,6 +803,12 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -830,7 +863,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -852,14 +885,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1181,10 +1218,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E93F6C7-E908-4D48-BE36-12E94BF6CA1A}">
-  <dimension ref="A1:M244"/>
+  <dimension ref="A1:M268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A203" zoomScale="92" workbookViewId="0">
-      <selection activeCell="C221" sqref="C221"/>
+    <sheetView topLeftCell="A235" zoomScale="92" workbookViewId="0">
+      <selection activeCell="E204" sqref="E204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="93.33203125" defaultRowHeight="15"/>
@@ -2140,7 +2177,7 @@
       </c>
     </row>
     <row r="121" spans="1:13">
-      <c r="A121" s="21" t="s">
+      <c r="A121" s="23" t="s">
         <v>89</v>
       </c>
       <c r="B121" s="3" t="s">
@@ -2150,7 +2187,7 @@
       <c r="M121" s="3"/>
     </row>
     <row r="122" spans="1:13">
-      <c r="A122" s="21"/>
+      <c r="A122" s="23"/>
       <c r="B122" s="3" t="s">
         <v>4</v>
       </c>
@@ -2162,7 +2199,7 @@
       </c>
     </row>
     <row r="123" spans="1:13" ht="16">
-      <c r="A123" s="21"/>
+      <c r="A123" s="23"/>
       <c r="B123" s="3" t="s">
         <v>5</v>
       </c>
@@ -2511,8 +2548,8 @@
       <c r="D173" s="3">
         <v>7.6438503265380797</v>
       </c>
-      <c r="E173" s="3" t="s">
-        <v>207</v>
+      <c r="E173" s="3">
+        <v>50</v>
       </c>
       <c r="H173" s="3" t="s">
         <v>199</v>
@@ -2521,7 +2558,7 @@
         <v>206</v>
       </c>
       <c r="J173" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="M173" s="3" t="s">
         <v>61</v>
@@ -2539,7 +2576,7 @@
       </c>
     </row>
     <row r="175" spans="1:13" ht="16">
-      <c r="A175" s="22" t="s">
+      <c r="A175" s="24" t="s">
         <v>172</v>
       </c>
       <c r="B175" s="3" t="s">
@@ -2549,7 +2586,7 @@
       <c r="M175" s="1"/>
     </row>
     <row r="176" spans="1:13">
-      <c r="A176" s="22"/>
+      <c r="A176" s="24"/>
       <c r="B176" s="3" t="s">
         <v>4</v>
       </c>
@@ -2664,27 +2701,27 @@
         <v>69</v>
       </c>
     </row>
-    <row r="193" spans="1:3">
+    <row r="193" spans="1:13">
       <c r="B193" s="5" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="194" spans="1:3">
+    <row r="194" spans="1:13">
       <c r="B194" s="5" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="195" spans="1:3">
+    <row r="195" spans="1:13">
       <c r="B195" s="15" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="196" spans="1:3" s="8" customFormat="1" ht="16" thickBot="1">
+    <row r="196" spans="1:13" s="8" customFormat="1" ht="16" thickBot="1">
       <c r="B196" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="197" spans="1:3">
+    <row r="197" spans="1:13">
       <c r="A197" s="3" t="s">
         <v>198</v>
       </c>
@@ -2694,125 +2731,181 @@
       <c r="C197" s="3">
         <v>93.376999999999995</v>
       </c>
-    </row>
-    <row r="198" spans="1:3" s="16" customFormat="1">
+      <c r="D197" s="25">
+        <v>3.8017436861991799E-2</v>
+      </c>
+      <c r="E197" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="H197" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="I197" s="25">
+        <v>7.3989787101745597</v>
+      </c>
+      <c r="J197" s="25">
+        <v>12.0481930673122</v>
+      </c>
+      <c r="M197" s="25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="198" spans="1:13" s="16" customFormat="1">
       <c r="B198" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="199" spans="1:3" s="16" customFormat="1">
+      <c r="H198" s="25" t="s">
+        <v>222</v>
+      </c>
+      <c r="M198" s="25" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="199" spans="1:13" s="16" customFormat="1" ht="16">
       <c r="B199" s="17" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="200" spans="1:3">
+      <c r="H199"/>
+      <c r="M199"/>
+    </row>
+    <row r="200" spans="1:13">
       <c r="B200" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="201" spans="1:3">
+      <c r="H200" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="M200" s="25" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="201" spans="1:13" ht="16">
       <c r="B201" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="202" spans="1:3">
+      <c r="H201"/>
+      <c r="M201"/>
+    </row>
+    <row r="202" spans="1:13">
       <c r="B202" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="203" spans="1:3">
+      <c r="H202" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="M202" s="25" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="203" spans="1:13" ht="16">
       <c r="B203" s="5" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="204" spans="1:3">
+      <c r="H203"/>
+      <c r="M203"/>
+    </row>
+    <row r="204" spans="1:13">
       <c r="B204" s="5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="205" spans="1:3">
+      <c r="H204" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="M204" s="25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="205" spans="1:13" ht="16">
       <c r="B205" s="5" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="206" spans="1:3">
+      <c r="H205"/>
+      <c r="M205"/>
+    </row>
+    <row r="206" spans="1:13">
       <c r="B206" s="5" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="207" spans="1:3">
+      <c r="H206" s="25" t="s">
+        <v>226</v>
+      </c>
+      <c r="M206" s="25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="207" spans="1:13">
       <c r="B207" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="208" spans="1:3">
+    <row r="208" spans="1:13">
       <c r="B208" s="5" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="209" spans="1:3">
+    <row r="209" spans="1:13">
       <c r="B209" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="210" spans="1:3">
+    <row r="210" spans="1:13">
       <c r="B210" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="211" spans="1:3">
+    <row r="211" spans="1:13">
       <c r="B211" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="212" spans="1:3">
+    <row r="212" spans="1:13">
       <c r="B212" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="213" spans="1:3">
+    <row r="213" spans="1:13">
       <c r="B213" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="214" spans="1:3">
+    <row r="214" spans="1:13">
       <c r="B214" s="5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="215" spans="1:3">
+    <row r="215" spans="1:13">
       <c r="B215" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="216" spans="1:3">
+    <row r="216" spans="1:13">
       <c r="B216" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="217" spans="1:3">
+    <row r="217" spans="1:13">
       <c r="B217" s="5" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="218" spans="1:3">
+    <row r="218" spans="1:13">
       <c r="B218" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="219" spans="1:3">
+    <row r="219" spans="1:13">
       <c r="B219" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="220" spans="1:3" s="8" customFormat="1" ht="16" thickBot="1">
+    <row r="220" spans="1:13" s="8" customFormat="1" ht="16" thickBot="1">
       <c r="B220" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="221" spans="1:3">
+    <row r="221" spans="1:13">
       <c r="A221" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B221" s="3" t="s">
         <v>169</v>
@@ -2820,141 +2913,326 @@
       <c r="C221" s="3">
         <v>37.889000000000003</v>
       </c>
-    </row>
-    <row r="222" spans="1:3">
+      <c r="F221" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="G221" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="H221" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="K221" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="L221" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="M221" s="25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="222" spans="1:13">
       <c r="B222" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="223" spans="1:3">
-      <c r="A223" s="22" t="s">
+      <c r="H222" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="M222" s="25" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="223" spans="1:13" ht="16">
+      <c r="A223" s="24" t="s">
         <v>172</v>
       </c>
       <c r="B223" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="224" spans="1:3">
-      <c r="A224" s="22"/>
+      <c r="H223"/>
+      <c r="M223"/>
+    </row>
+    <row r="224" spans="1:13">
+      <c r="A224" s="24"/>
       <c r="B224" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="225" spans="1:2">
+      <c r="H224" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="M224" s="25" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="225" spans="1:13" ht="16">
       <c r="B225" s="5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="226" spans="1:2">
-      <c r="A226" s="23" t="s">
-        <v>210</v>
+      <c r="H225"/>
+      <c r="M225"/>
+    </row>
+    <row r="226" spans="1:13">
+      <c r="A226" s="21" t="s">
+        <v>209</v>
       </c>
       <c r="B226" s="5" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="227" spans="1:2">
-      <c r="A227" s="22" t="s">
-        <v>211</v>
+      <c r="H226" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="M226" s="25" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="227" spans="1:13" ht="16">
+      <c r="A227" s="24" t="s">
+        <v>210</v>
       </c>
       <c r="B227" s="5" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="228" spans="1:2">
-      <c r="A228" s="22"/>
+      <c r="H227"/>
+      <c r="M227"/>
+    </row>
+    <row r="228" spans="1:13">
+      <c r="A228" s="24"/>
       <c r="B228" s="5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="229" spans="1:2">
+      <c r="H228" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="M228" s="25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="229" spans="1:13" ht="16">
       <c r="B229" s="5" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="230" spans="1:2">
+      <c r="H229"/>
+      <c r="M229"/>
+    </row>
+    <row r="230" spans="1:13">
       <c r="B230" s="5" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="231" spans="1:2">
+      <c r="H230" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="M230" s="25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="231" spans="1:13">
       <c r="B231" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="232" spans="1:2">
+    <row r="232" spans="1:13">
       <c r="B232" s="5" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="233" spans="1:2">
+    <row r="233" spans="1:13">
       <c r="B233" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="234" spans="1:2">
+    <row r="234" spans="1:13">
       <c r="B234" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="235" spans="1:2">
+    <row r="235" spans="1:13">
       <c r="B235" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="236" spans="1:2">
+    <row r="236" spans="1:13">
       <c r="B236" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="237" spans="1:2">
+    <row r="237" spans="1:13">
       <c r="B237" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="238" spans="1:2">
+    <row r="238" spans="1:13">
       <c r="B238" s="5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="239" spans="1:2">
+    <row r="239" spans="1:13">
       <c r="B239" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="240" spans="1:2">
+    <row r="240" spans="1:13">
       <c r="B240" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="241" spans="2:2">
+    <row r="241" spans="1:2">
       <c r="B241" s="5" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="242" spans="2:2">
+    <row r="242" spans="1:2">
       <c r="B242" s="5" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="243" spans="2:2">
+    <row r="243" spans="1:2">
       <c r="B243" s="15" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="244" spans="2:2" s="8" customFormat="1" ht="16" thickBot="1">
+    <row r="244" spans="1:2" s="8" customFormat="1" ht="16" thickBot="1">
       <c r="B244" s="4" t="s">
         <v>20</v>
       </c>
     </row>
+    <row r="245" spans="1:2">
+      <c r="A245" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="B245" s="19" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2">
+      <c r="B246" s="19" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2">
+      <c r="A247" s="26" t="s">
+        <v>232</v>
+      </c>
+      <c r="B247" s="19" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2">
+      <c r="A248" s="26"/>
+      <c r="B248" s="19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2">
+      <c r="A249" s="26"/>
+      <c r="B249" s="19" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2">
+      <c r="B250" s="19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2">
+      <c r="B251" s="19" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2">
+      <c r="B252" s="19" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2">
+      <c r="B253" s="19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2">
+      <c r="B254" s="19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2">
+      <c r="B255" s="20" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2">
+      <c r="B256" s="20" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="257" spans="2:2">
+      <c r="B257" s="20" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="258" spans="2:2">
+      <c r="B258" s="20" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="259" spans="2:2">
+      <c r="B259" s="20" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="260" spans="2:2">
+      <c r="B260" s="20" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="261" spans="2:2">
+      <c r="B261" s="20" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="262" spans="2:2">
+      <c r="B262" s="19" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="263" spans="2:2">
+      <c r="B263" s="19" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="264" spans="2:2">
+      <c r="B264" s="19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="265" spans="2:2">
+      <c r="B265" s="19" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="266" spans="2:2">
+      <c r="B266" s="19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="267" spans="2:2">
+      <c r="B267" s="19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="268" spans="2:2" s="8" customFormat="1" ht="16" thickBot="1">
+      <c r="B268" s="22" t="s">
+        <v>114</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A121:A123"/>
     <mergeCell ref="A175:A176"/>
     <mergeCell ref="A223:A224"/>
     <mergeCell ref="A227:A228"/>
+    <mergeCell ref="A247:A249"/>
   </mergeCells>
-  <conditionalFormatting sqref="E10:E37 E93:E118 E120:E145 E157:E172 E39:E91 E174:E1048576">
+  <conditionalFormatting sqref="E10:E37 E93:E118 E120:E145 E157:E172 E39:E91 E174:E196 E198:E1048576">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -2964,7 +3242,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E10:E37 E120:E145 E157:E172 E39:E118 E174:E1048576">
+  <conditionalFormatting sqref="E10:E37 E120:E145 E157:E172 E39:E118 E174:E196 E198:E1048576">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -2984,7 +3262,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J11:J37 J157:J172 J39:J145 J174:J263">
+  <conditionalFormatting sqref="J11:J37 J157:J172 J39:J145 J174:J196 J198:J263">
     <cfRule type="colorScale" priority="51">
       <colorScale>
         <cfvo type="min"/>
@@ -2994,7 +3272,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J11:J172 J174:J802">
+  <conditionalFormatting sqref="J11:J172 J174:J196 J198:J802">
     <cfRule type="colorScale" priority="55">
       <colorScale>
         <cfvo type="min"/>
@@ -3004,7 +3282,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E11:E172 E174:E922">
+  <conditionalFormatting sqref="E11:E172 E174:E196 E198:E922">
     <cfRule type="colorScale" priority="57">
       <colorScale>
         <cfvo type="min"/>
@@ -3014,7 +3292,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J11:J1048576 J1:J9">
+  <conditionalFormatting sqref="J11:J196 J1:J9 J198:J1048576">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -3032,8 +3310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EF8B63F-B594-7045-961A-3C8367EEFC3D}">
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3149,8 +3427,8 @@
       <c r="D11" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>182</v>
+      <c r="E11" s="1">
+        <v>50</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>183</v>
@@ -3345,19 +3623,19 @@
         <v>197</v>
       </c>
       <c r="D39" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E39" s="1">
+        <v>80.174999999999997</v>
+      </c>
+      <c r="H39" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="E39" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>214</v>
-      </c>
       <c r="I39" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="J39" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
+      </c>
+      <c r="J39" s="1">
+        <v>69.879519939422593</v>
       </c>
       <c r="M39" s="1" t="s">
         <v>44</v>
@@ -3368,10 +3646,10 @@
         <v>115</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="41" spans="1:13">
@@ -3390,10 +3668,10 @@
         <v>116</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="43" spans="1:13">
@@ -3401,10 +3679,10 @@
         <v>117</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="44" spans="1:13">
@@ -3412,7 +3690,7 @@
         <v>118</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="M44" s="1" t="s">
         <v>47</v>
@@ -3423,7 +3701,7 @@
         <v>119</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="M45" s="1" t="s">
         <v>193</v>
@@ -3515,7 +3793,7 @@
       </c>
     </row>
     <row r="63" spans="2:2" s="2" customFormat="1" ht="17" thickBot="1">
-      <c r="B63" s="24" t="s">
+      <c r="B63" s="22" t="s">
         <v>114</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Referting changes back to one of my first CNNs
</commit_message>
<xml_diff>
--- a/ArchitectureResults.xlsx
+++ b/ArchitectureResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annarienbester/git/gravitationallenses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B71863-36C9-0C42-BC0E-66F5885904E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75126F2C-DDB5-7644-8E1F-7771997F54D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{732A71FF-1E05-B648-932B-29EDA13B68A3}"/>
+    <workbookView xWindow="280" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{732A71FF-1E05-B648-932B-29EDA13B68A3}"/>
   </bookViews>
   <sheets>
     <sheet name="OnHep" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="236">
   <si>
     <t>DATE</t>
   </si>
@@ -730,13 +730,19 @@
     <t>1.0</t>
   </si>
   <si>
-    <t>31_10_2020_07_24_19</t>
-  </si>
-  <si>
     <t>Running the one from my laptop on hep, with k=5</t>
   </si>
   <si>
     <t> 98,75704050064087</t>
+  </si>
+  <si>
+    <t>31_10_2020_11_31_55</t>
+  </si>
+  <si>
+    <t>31_10_2020_15_34_55</t>
+  </si>
+  <si>
+    <t>Running without data augmentation, no k fold, to see if with less data results improve</t>
   </si>
 </sst>
 </file>
@@ -746,7 +752,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -803,12 +809,6 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Menlo"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -863,7 +863,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -893,7 +893,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1218,26 +1217,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E93F6C7-E908-4D48-BE36-12E94BF6CA1A}">
-  <dimension ref="A1:M268"/>
+  <dimension ref="A1:M292"/>
   <sheetViews>
-    <sheetView topLeftCell="A235" zoomScale="92" workbookViewId="0">
-      <selection activeCell="E204" sqref="E204"/>
+    <sheetView tabSelected="1" topLeftCell="A259" zoomScale="92" workbookViewId="0">
+      <selection activeCell="A276" sqref="A276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="93.33203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="91" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="22.6640625" style="6" customWidth="1"/>
-    <col min="11" max="11" width="18.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="85.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.83203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="18" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="12.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23" style="6" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="54" style="6" customWidth="1"/>
     <col min="15" max="16384" width="93.33203125" style="6"/>
   </cols>
@@ -2731,22 +2728,22 @@
       <c r="C197" s="3">
         <v>93.376999999999995</v>
       </c>
-      <c r="D197" s="25">
+      <c r="D197" s="3">
         <v>3.8017436861991799E-2</v>
       </c>
-      <c r="E197" s="25" t="s">
-        <v>233</v>
-      </c>
-      <c r="H197" s="25" t="s">
+      <c r="E197" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="H197" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="I197" s="25">
+      <c r="I197" s="3">
         <v>7.3989787101745597</v>
       </c>
-      <c r="J197" s="25">
+      <c r="J197" s="3">
         <v>12.0481930673122</v>
       </c>
-      <c r="M197" s="25" t="s">
+      <c r="M197" s="3" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2754,10 +2751,10 @@
       <c r="B198" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H198" s="25" t="s">
+      <c r="H198" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="M198" s="25" t="s">
+      <c r="M198" s="3" t="s">
         <v>227</v>
       </c>
     </row>
@@ -2765,17 +2762,17 @@
       <c r="B199" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="H199"/>
-      <c r="M199"/>
+      <c r="H199" s="1"/>
+      <c r="M199" s="1"/>
     </row>
     <row r="200" spans="1:13">
       <c r="B200" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H200" s="25" t="s">
+      <c r="H200" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="M200" s="25" t="s">
+      <c r="M200" s="3" t="s">
         <v>228</v>
       </c>
     </row>
@@ -2783,17 +2780,17 @@
       <c r="B201" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H201"/>
-      <c r="M201"/>
+      <c r="H201" s="1"/>
+      <c r="M201" s="1"/>
     </row>
     <row r="202" spans="1:13">
       <c r="B202" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H202" s="25" t="s">
+      <c r="H202" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="M202" s="25" t="s">
+      <c r="M202" s="3" t="s">
         <v>229</v>
       </c>
     </row>
@@ -2801,17 +2798,17 @@
       <c r="B203" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="H203"/>
-      <c r="M203"/>
+      <c r="H203" s="1"/>
+      <c r="M203" s="1"/>
     </row>
     <row r="204" spans="1:13">
       <c r="B204" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="H204" s="25" t="s">
+      <c r="H204" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="M204" s="25" t="s">
+      <c r="M204" s="3" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2819,17 +2816,17 @@
       <c r="B205" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="H205"/>
-      <c r="M205"/>
+      <c r="H205" s="1"/>
+      <c r="M205" s="1"/>
     </row>
     <row r="206" spans="1:13">
       <c r="B206" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="H206" s="25" t="s">
+      <c r="H206" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="M206" s="25" t="s">
+      <c r="M206" s="3" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2919,7 +2916,7 @@
       <c r="G221" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="H221" s="25" t="s">
+      <c r="H221" s="3" t="s">
         <v>199</v>
       </c>
       <c r="K221" s="6" t="s">
@@ -2928,7 +2925,7 @@
       <c r="L221" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="M221" s="25" t="s">
+      <c r="M221" s="3" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2936,10 +2933,10 @@
       <c r="B222" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H222" s="25" t="s">
+      <c r="H222" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="M222" s="25" t="s">
+      <c r="M222" s="3" t="s">
         <v>204</v>
       </c>
     </row>
@@ -2950,18 +2947,18 @@
       <c r="B223" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H223"/>
-      <c r="M223"/>
+      <c r="H223" s="1"/>
+      <c r="M223" s="1"/>
     </row>
     <row r="224" spans="1:13">
       <c r="A224" s="24"/>
       <c r="B224" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H224" s="25" t="s">
+      <c r="H224" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="M224" s="25" t="s">
+      <c r="M224" s="3" t="s">
         <v>205</v>
       </c>
     </row>
@@ -2969,8 +2966,8 @@
       <c r="B225" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="H225"/>
-      <c r="M225"/>
+      <c r="H225" s="1"/>
+      <c r="M225" s="1"/>
     </row>
     <row r="226" spans="1:13">
       <c r="A226" s="21" t="s">
@@ -2979,10 +2976,10 @@
       <c r="B226" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="H226" s="25" t="s">
+      <c r="H226" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="M226" s="25" t="s">
+      <c r="M226" s="3" t="s">
         <v>202</v>
       </c>
     </row>
@@ -2993,18 +2990,18 @@
       <c r="B227" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="H227"/>
-      <c r="M227"/>
+      <c r="H227" s="1"/>
+      <c r="M227" s="1"/>
     </row>
     <row r="228" spans="1:13">
       <c r="A228" s="24"/>
       <c r="B228" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="H228" s="25" t="s">
+      <c r="H228" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="M228" s="25" t="s">
+      <c r="M228" s="3" t="s">
         <v>65</v>
       </c>
     </row>
@@ -3012,17 +3009,17 @@
       <c r="B229" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="H229"/>
-      <c r="M229"/>
+      <c r="H229" s="1"/>
+      <c r="M229" s="1"/>
     </row>
     <row r="230" spans="1:13">
       <c r="B230" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="H230" s="25" t="s">
+      <c r="H230" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="M230" s="25" t="s">
+      <c r="M230" s="3" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3076,164 +3073,300 @@
         <v>69</v>
       </c>
     </row>
-    <row r="241" spans="1:2">
+    <row r="241" spans="1:3">
       <c r="B241" s="5" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="242" spans="1:2">
+    <row r="242" spans="1:3">
       <c r="B242" s="5" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="243" spans="1:2">
+    <row r="243" spans="1:3">
       <c r="B243" s="15" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="244" spans="1:2" s="8" customFormat="1" ht="16" thickBot="1">
+    <row r="244" spans="1:3" s="8" customFormat="1" ht="16" thickBot="1">
       <c r="B244" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="245" spans="1:2">
-      <c r="A245" s="6" t="s">
+    <row r="245" spans="1:3">
+      <c r="A245" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="B245" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="C245" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3">
+      <c r="B246" s="12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3">
+      <c r="A247" s="25" t="s">
         <v>231</v>
       </c>
-      <c r="B245" s="19" t="s">
+      <c r="B247" s="12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3">
+      <c r="A248" s="25"/>
+      <c r="B248" s="12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3">
+      <c r="A249" s="25"/>
+      <c r="B249" s="12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3">
+      <c r="B250" s="12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3">
+      <c r="B251" s="12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3">
+      <c r="B252" s="12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3">
+      <c r="B253" s="12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3">
+      <c r="B254" s="12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3">
+      <c r="B255" s="14" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3">
+      <c r="B256" s="14" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3">
+      <c r="B257" s="14" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3">
+      <c r="B258" s="14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3">
+      <c r="B259" s="14" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3">
+      <c r="B260" s="14" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3">
+      <c r="B261" s="14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3">
+      <c r="B262" s="12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3">
+      <c r="B263" s="12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3">
+      <c r="B264" s="12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3">
+      <c r="B265" s="12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3">
+      <c r="B266" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3">
+      <c r="B267" s="12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" s="8" customFormat="1" ht="16" thickBot="1">
+      <c r="B268" s="13" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3">
+      <c r="A269" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="B269" s="12" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="246" spans="1:2">
-      <c r="B246" s="19" t="s">
+      <c r="C269" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3">
+      <c r="B270" s="12" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="247" spans="1:2">
-      <c r="A247" s="26" t="s">
-        <v>232</v>
-      </c>
-      <c r="B247" s="19" t="s">
+    <row r="271" spans="1:3" ht="15" customHeight="1">
+      <c r="A271" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="B271" s="12" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="248" spans="1:2">
-      <c r="A248" s="26"/>
-      <c r="B248" s="19" t="s">
+    <row r="272" spans="1:3">
+      <c r="A272" s="25"/>
+      <c r="B272" s="12" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="249" spans="1:2">
-      <c r="A249" s="26"/>
-      <c r="B249" s="19" t="s">
+    <row r="273" spans="1:2">
+      <c r="A273" s="25"/>
+      <c r="B273" s="12" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="250" spans="1:2">
-      <c r="B250" s="19" t="s">
+    <row r="274" spans="1:2">
+      <c r="A274" s="25"/>
+      <c r="B274" s="12" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="251" spans="1:2">
-      <c r="B251" s="19" t="s">
+    <row r="275" spans="1:2">
+      <c r="B275" s="12" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="252" spans="1:2">
-      <c r="B252" s="19" t="s">
+    <row r="276" spans="1:2">
+      <c r="B276" s="12" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="253" spans="1:2">
-      <c r="B253" s="19" t="s">
+    <row r="277" spans="1:2">
+      <c r="B277" s="12" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="254" spans="1:2">
-      <c r="B254" s="19" t="s">
+    <row r="278" spans="1:2">
+      <c r="B278" s="12" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="255" spans="1:2">
-      <c r="B255" s="20" t="s">
+    <row r="279" spans="1:2">
+      <c r="B279" s="14" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="256" spans="1:2">
-      <c r="B256" s="20" t="s">
+    <row r="280" spans="1:2">
+      <c r="B280" s="14" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="257" spans="2:2">
-      <c r="B257" s="20" t="s">
+    <row r="281" spans="1:2">
+      <c r="B281" s="14" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="258" spans="2:2">
-      <c r="B258" s="20" t="s">
+    <row r="282" spans="1:2">
+      <c r="B282" s="14" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="259" spans="2:2">
-      <c r="B259" s="20" t="s">
+    <row r="283" spans="1:2">
+      <c r="B283" s="14" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="260" spans="2:2">
-      <c r="B260" s="20" t="s">
+    <row r="284" spans="1:2">
+      <c r="B284" s="14" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="261" spans="2:2">
-      <c r="B261" s="20" t="s">
+    <row r="285" spans="1:2">
+      <c r="B285" s="14" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="262" spans="2:2">
-      <c r="B262" s="19" t="s">
+    <row r="286" spans="1:2">
+      <c r="B286" s="12" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="263" spans="2:2">
-      <c r="B263" s="19" t="s">
+    <row r="287" spans="1:2">
+      <c r="B287" s="12" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="264" spans="2:2">
-      <c r="B264" s="19" t="s">
+    <row r="288" spans="1:2">
+      <c r="B288" s="12" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="265" spans="2:2">
-      <c r="B265" s="19" t="s">
+    <row r="289" spans="2:2">
+      <c r="B289" s="12" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="266" spans="2:2">
-      <c r="B266" s="19" t="s">
+    <row r="290" spans="2:2">
+      <c r="B290" s="12" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="267" spans="2:2">
-      <c r="B267" s="19" t="s">
+    <row r="291" spans="2:2">
+      <c r="B291" s="12" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="268" spans="2:2" s="8" customFormat="1" ht="16" thickBot="1">
-      <c r="B268" s="22" t="s">
+    <row r="292" spans="2:2" s="8" customFormat="1" ht="16" thickBot="1">
+      <c r="B292" s="13" t="s">
         <v>114</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A271:A274"/>
     <mergeCell ref="A121:A123"/>
     <mergeCell ref="A175:A176"/>
     <mergeCell ref="A223:A224"/>
     <mergeCell ref="A227:A228"/>
     <mergeCell ref="A247:A249"/>
   </mergeCells>
-  <conditionalFormatting sqref="E10:E37 E93:E118 E120:E145 E157:E172 E39:E91 E174:E196 E198:E1048576">
-    <cfRule type="colorScale" priority="18">
+  <conditionalFormatting sqref="E10:E37 E93:E118 E120:E145 E157:E172 E39:E91 E174:E196 E198:E268 E293:E1048576">
+    <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3242,8 +3375,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E10:E37 E120:E145 E157:E172 E39:E118 E174:E196 E198:E1048576">
-    <cfRule type="colorScale" priority="23">
+  <conditionalFormatting sqref="E10:E37 E120:E145 E157:E172 E39:E118 E174:E196 E198:E268 E293:E1048576">
+    <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3251,7 +3384,7 @@
         <color rgb="FF92D050"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="24">
+    <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3263,7 +3396,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:J37 J157:J172 J39:J145 J174:J196 J198:J263">
-    <cfRule type="colorScale" priority="51">
+    <cfRule type="colorScale" priority="58">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3272,8 +3405,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J11:J172 J174:J196 J198:J802">
-    <cfRule type="colorScale" priority="55">
+  <conditionalFormatting sqref="J11:J172 J174:J196 J198:J268 J293:J802">
+    <cfRule type="colorScale" priority="62">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3282,8 +3415,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E11:E172 E174:E196 E198:E922">
-    <cfRule type="colorScale" priority="57">
+  <conditionalFormatting sqref="E11:E172 E174:E196 E198:E268 E293:E922">
+    <cfRule type="colorScale" priority="64">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3292,7 +3425,77 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J11:J196 J1:J9 J198:J1048576">
+  <conditionalFormatting sqref="J11:J196 J1:J9 J198:J268 J293:J1048576">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FF92D050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E269:E292">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFA836F"/>
+        <color theme="9" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E269:E292">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFA836F"/>
+        <color rgb="FF92D050"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J269:J287">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFA836F"/>
+        <color theme="9" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J269:J292">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF89890"/>
+        <color rgb="FF92D050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E269:E292">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF89890"/>
+        <color theme="9" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J269:J292">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -3310,8 +3513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EF8B63F-B594-7045-961A-3C8367EEFC3D}">
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>